<commit_message>
selesai sampai warna pink
</commit_message>
<xml_diff>
--- a/kamila_sarimbit shafeeya.xlsx
+++ b/kamila_sarimbit shafeeya.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\sarimbit-shafeeya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3440766E-9F65-468A-81F3-2B64473E640F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74B4A53-A26C-47AF-950D-4EDB57544EE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="103">
   <si>
     <t>Timestamp</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Koko Anak Maroon- XS</t>
-  </si>
-  <si>
-    <t>Koko Anak Maroon - S</t>
   </si>
   <si>
     <t>Koko Anak Maroon- M</t>
@@ -347,7 +344,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -546,13 +543,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -593,18 +590,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,6 +601,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -892,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:E15547"/>
+  <dimension ref="A3:E15526"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -943,7 +940,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="23"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -956,7 +953,7 @@
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="23"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
@@ -969,7 +966,7 @@
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="23"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
@@ -982,7 +979,7 @@
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="23"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -995,7 +992,7 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="24"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1008,7 +1005,7 @@
       <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="24"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1021,7 +1018,7 @@
       <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="24"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1034,7 +1031,7 @@
       <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="24"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1047,7 +1044,7 @@
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="24"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
@@ -1060,7 +1057,7 @@
       <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="24"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -1073,7 +1070,7 @@
       <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="24"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1086,7 +1083,7 @@
       <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="24"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1099,12 +1096,12 @@
       <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="24"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="12">
         <v>0</v>
@@ -1112,7 +1109,7 @@
       <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="24"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1125,20 +1122,20 @@
       <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="24"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="11">
+        <v>0</v>
+      </c>
+      <c r="D21" s="12">
         <v>1</v>
       </c>
-      <c r="D21" s="12">
-        <v>0</v>
-      </c>
       <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="24"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="5" t="s">
         <v>22</v>
       </c>
@@ -1151,7 +1148,7 @@
       <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="24"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
@@ -1164,33 +1161,33 @@
       <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="24"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="11">
+        <v>1</v>
+      </c>
+      <c r="D24" s="12">
         <v>0</v>
       </c>
-      <c r="D24" s="12">
-        <v>1</v>
-      </c>
       <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="24"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="24"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="5" t="s">
         <v>26</v>
       </c>
@@ -1203,7 +1200,7 @@
       <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="25"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="5" t="s">
         <v>27</v>
       </c>
@@ -1216,7 +1213,7 @@
       <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="25"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="5" t="s">
         <v>28</v>
       </c>
@@ -1229,7 +1226,7 @@
       <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="25"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="5" t="s">
         <v>29</v>
       </c>
@@ -1242,7 +1239,7 @@
       <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="25"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="5" t="s">
         <v>30</v>
       </c>
@@ -1250,12 +1247,12 @@
         <v>0</v>
       </c>
       <c r="D30" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="26"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
@@ -1268,7 +1265,7 @@
       <c r="E31" s="10"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="26"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
@@ -1281,7 +1278,7 @@
       <c r="E32" s="10"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="26"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="5" t="s">
         <v>33</v>
       </c>
@@ -1289,12 +1286,12 @@
         <v>0</v>
       </c>
       <c r="D33" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="10"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="26"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="5" t="s">
         <v>34</v>
       </c>
@@ -1302,12 +1299,12 @@
         <v>0</v>
       </c>
       <c r="D34" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="10"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="27"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="5" t="s">
         <v>35</v>
       </c>
@@ -1320,46 +1317,46 @@
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="27"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C36" s="11">
+        <v>3</v>
+      </c>
+      <c r="D36" s="12">
         <v>0</v>
       </c>
-      <c r="D36" s="12">
-        <v>1</v>
-      </c>
       <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="27"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C37" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D37" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="27"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C38" s="11">
+        <v>0</v>
+      </c>
+      <c r="D38" s="12">
         <v>1</v>
       </c>
-      <c r="D38" s="12">
-        <v>2</v>
-      </c>
       <c r="E38" s="10"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="27"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="5" t="s">
         <v>39</v>
       </c>
@@ -1367,38 +1364,38 @@
         <v>0</v>
       </c>
       <c r="D39" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="10"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="27"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C40" s="11">
+        <v>1</v>
+      </c>
+      <c r="D40" s="12">
         <v>0</v>
       </c>
-      <c r="D40" s="12">
-        <v>2</v>
-      </c>
       <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="27"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C41" s="11">
+        <v>0</v>
+      </c>
+      <c r="D41" s="12">
         <v>1</v>
       </c>
-      <c r="D41" s="12">
-        <v>0</v>
-      </c>
       <c r="E41" s="10"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="27"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="5" t="s">
         <v>42</v>
       </c>
@@ -1406,12 +1403,12 @@
         <v>0</v>
       </c>
       <c r="D42" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="27"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="5" t="s">
         <v>43</v>
       </c>
@@ -1419,30 +1416,30 @@
         <v>0</v>
       </c>
       <c r="D43" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="27"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C44" s="11">
+        <v>1</v>
+      </c>
+      <c r="D44" s="12">
         <v>0</v>
       </c>
-      <c r="D44" s="12">
-        <v>1</v>
-      </c>
       <c r="E44" s="10"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="27"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C45" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" s="12">
         <v>0</v>
@@ -1450,20 +1447,20 @@
       <c r="E45" s="10"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="27"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C46" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D46" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="10"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="28"/>
+      <c r="A47" s="24"/>
       <c r="B47" s="5" t="s">
         <v>49</v>
       </c>
@@ -1471,12 +1468,12 @@
         <v>0</v>
       </c>
       <c r="D47" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E47" s="10"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="28"/>
+      <c r="A48" s="24"/>
       <c r="B48" s="5" t="s">
         <v>50</v>
       </c>
@@ -1489,22 +1486,22 @@
       <c r="E48" s="10"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="28"/>
+      <c r="A49" s="24"/>
       <c r="B49" s="5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C49" s="11">
         <v>0</v>
       </c>
       <c r="D49" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" s="10"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="28"/>
+      <c r="A50" s="24"/>
       <c r="B50" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C50" s="11">
         <v>0</v>
@@ -1515,9 +1512,9 @@
       <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="28"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C51" s="11">
         <v>0</v>
@@ -1528,9 +1525,9 @@
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="28"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="5" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C52" s="11">
         <v>0</v>
@@ -1541,7 +1538,7 @@
       <c r="E52" s="10"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="28"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="5" t="s">
         <v>77</v>
       </c>
@@ -1554,9 +1551,9 @@
       <c r="E53" s="10"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="28"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C54" s="11">
         <v>0</v>
@@ -1567,22 +1564,24 @@
       <c r="E54" s="10"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="28"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="5" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C55" s="11">
         <v>0</v>
       </c>
       <c r="D55" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" s="10"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="28"/>
+      <c r="A56" s="25" t="s">
+        <v>99</v>
+      </c>
       <c r="B56" s="5" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="C56" s="11">
         <v>0</v>
@@ -1593,9 +1592,9 @@
       <c r="E56" s="10"/>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="28"/>
+      <c r="A57" s="25"/>
       <c r="B57" s="5" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="C57" s="11">
         <v>0</v>
@@ -1606,9 +1605,9 @@
       <c r="E57" s="10"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="28"/>
+      <c r="A58" s="25"/>
       <c r="B58" s="5" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="C58" s="11">
         <v>0</v>
@@ -1619,9 +1618,9 @@
       <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="28"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="5" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="C59" s="11">
         <v>0</v>
@@ -1632,22 +1631,22 @@
       <c r="E59" s="10"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="28"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="5" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C60" s="11">
         <v>0</v>
       </c>
       <c r="D60" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" s="10"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="28"/>
+      <c r="A61" s="25"/>
       <c r="B61" s="5" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C61" s="11">
         <v>0</v>
@@ -1658,9 +1657,9 @@
       <c r="E61" s="10"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="28"/>
+      <c r="A62" s="25"/>
       <c r="B62" s="5" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C62" s="11">
         <v>0</v>
@@ -1671,9 +1670,9 @@
       <c r="E62" s="10"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="28"/>
+      <c r="A63" s="25"/>
       <c r="B63" s="5" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C63" s="11">
         <v>0</v>
@@ -1684,9 +1683,9 @@
       <c r="E63" s="10"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="28"/>
+      <c r="A64" s="25"/>
       <c r="B64" s="5" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="C64" s="11">
         <v>0</v>
@@ -1697,9 +1696,9 @@
       <c r="E64" s="10"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="28"/>
+      <c r="A65" s="25"/>
       <c r="B65" s="5" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="C65" s="11">
         <v>0</v>
@@ -1710,9 +1709,9 @@
       <c r="E65" s="10"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="28"/>
+      <c r="A66" s="25"/>
       <c r="B66" s="5" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="C66" s="11">
         <v>0</v>
@@ -1723,22 +1722,22 @@
       <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="28"/>
+      <c r="A67" s="25"/>
       <c r="B67" s="5" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="C67" s="11">
         <v>0</v>
       </c>
       <c r="D67" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="28"/>
+      <c r="A68" s="25"/>
       <c r="B68" s="5" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C68" s="11">
         <v>0</v>
@@ -1749,9 +1748,9 @@
       <c r="E68" s="10"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="28"/>
+      <c r="A69" s="25"/>
       <c r="B69" s="5" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="C69" s="11">
         <v>0</v>
@@ -1762,9 +1761,9 @@
       <c r="E69" s="10"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="28"/>
+      <c r="A70" s="25"/>
       <c r="B70" s="5" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="C70" s="11">
         <v>0</v>
@@ -1775,9 +1774,9 @@
       <c r="E70" s="10"/>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="28"/>
+      <c r="A71" s="25"/>
       <c r="B71" s="5" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C71" s="11">
         <v>0</v>
@@ -1788,9 +1787,9 @@
       <c r="E71" s="10"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="28"/>
+      <c r="A72" s="25"/>
       <c r="B72" s="5" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="C72" s="11">
         <v>0</v>
@@ -1801,9 +1800,9 @@
       <c r="E72" s="10"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="28"/>
+      <c r="A73" s="25"/>
       <c r="B73" s="5" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="C73" s="11">
         <v>0</v>
@@ -1814,9 +1813,9 @@
       <c r="E73" s="10"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="28"/>
+      <c r="A74" s="25"/>
       <c r="B74" s="5" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="C74" s="11">
         <v>0</v>
@@ -1827,9 +1826,9 @@
       <c r="E74" s="10"/>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="28"/>
+      <c r="A75" s="25"/>
       <c r="B75" s="5" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="C75" s="11">
         <v>0</v>
@@ -1840,9 +1839,9 @@
       <c r="E75" s="10"/>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="28"/>
+      <c r="A76" s="25"/>
       <c r="B76" s="5" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="C76" s="11">
         <v>0</v>
@@ -1853,11 +1852,9 @@
       <c r="E76" s="10"/>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="29" t="s">
-        <v>100</v>
-      </c>
+      <c r="A77" s="25"/>
       <c r="B77" s="5" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C77" s="11">
         <v>0</v>
@@ -1868,9 +1865,9 @@
       <c r="E77" s="10"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="29"/>
+      <c r="A78" s="25"/>
       <c r="B78" s="5" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C78" s="11">
         <v>0</v>
@@ -1881,9 +1878,9 @@
       <c r="E78" s="10"/>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="29"/>
+      <c r="A79" s="25"/>
       <c r="B79" s="5" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C79" s="11">
         <v>0</v>
@@ -1894,9 +1891,9 @@
       <c r="E79" s="10"/>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="29"/>
+      <c r="A80" s="25"/>
       <c r="B80" s="5" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C80" s="11">
         <v>0</v>
@@ -1907,9 +1904,9 @@
       <c r="E80" s="10"/>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="29"/>
+      <c r="A81" s="25"/>
       <c r="B81" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C81" s="11">
         <v>0</v>
@@ -1920,9 +1917,9 @@
       <c r="E81" s="10"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="29"/>
+      <c r="A82" s="25"/>
       <c r="B82" s="5" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="C82" s="11">
         <v>0</v>
@@ -1933,9 +1930,9 @@
       <c r="E82" s="10"/>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="29"/>
+      <c r="A83" s="25"/>
       <c r="B83" s="5" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C83" s="11">
         <v>0</v>
@@ -1946,9 +1943,9 @@
       <c r="E83" s="10"/>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="29"/>
+      <c r="A84" s="25"/>
       <c r="B84" s="5" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C84" s="11">
         <v>0</v>
@@ -1959,9 +1956,9 @@
       <c r="E84" s="10"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="29"/>
+      <c r="A85" s="25"/>
       <c r="B85" s="5" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="C85" s="11">
         <v>0</v>
@@ -1972,9 +1969,9 @@
       <c r="E85" s="10"/>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="29"/>
+      <c r="A86" s="25"/>
       <c r="B86" s="5" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C86" s="11">
         <v>0</v>
@@ -1985,9 +1982,9 @@
       <c r="E86" s="10"/>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="29"/>
+      <c r="A87" s="25"/>
       <c r="B87" s="5" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C87" s="11">
         <v>0</v>
@@ -1998,9 +1995,9 @@
       <c r="E87" s="10"/>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="29"/>
+      <c r="A88" s="25"/>
       <c r="B88" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C88" s="11">
         <v>0</v>
@@ -2011,9 +2008,9 @@
       <c r="E88" s="10"/>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="29"/>
+      <c r="A89" s="25"/>
       <c r="B89" s="5" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C89" s="11">
         <v>0</v>
@@ -2024,9 +2021,9 @@
       <c r="E89" s="10"/>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="29"/>
+      <c r="A90" s="25"/>
       <c r="B90" s="5" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C90" s="11">
         <v>0</v>
@@ -2037,9 +2034,9 @@
       <c r="E90" s="10"/>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="29"/>
+      <c r="A91" s="25"/>
       <c r="B91" s="5" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C91" s="11">
         <v>0</v>
@@ -2050,9 +2047,9 @@
       <c r="E91" s="10"/>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="29"/>
+      <c r="A92" s="25"/>
       <c r="B92" s="5" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C92" s="11">
         <v>0</v>
@@ -2063,9 +2060,9 @@
       <c r="E92" s="10"/>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="29"/>
+      <c r="A93" s="25"/>
       <c r="B93" s="5" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C93" s="11">
         <v>0</v>
@@ -2076,9 +2073,9 @@
       <c r="E93" s="10"/>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="29"/>
+      <c r="A94" s="25"/>
       <c r="B94" s="5" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C94" s="11">
         <v>0</v>
@@ -2089,9 +2086,9 @@
       <c r="E94" s="10"/>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="29"/>
+      <c r="A95" s="25"/>
       <c r="B95" s="5" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C95" s="11">
         <v>0</v>
@@ -2102,9 +2099,9 @@
       <c r="E95" s="10"/>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="29"/>
+      <c r="A96" s="25"/>
       <c r="B96" s="5" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="C96" s="11">
         <v>0</v>
@@ -2115,9 +2112,9 @@
       <c r="E96" s="10"/>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="29"/>
+      <c r="A97" s="25"/>
       <c r="B97" s="5" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="C97" s="11">
         <v>0</v>
@@ -2128,9 +2125,9 @@
       <c r="E97" s="10"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="29"/>
+      <c r="A98" s="25"/>
       <c r="B98" s="5" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="C98" s="11">
         <v>0</v>
@@ -2141,9 +2138,9 @@
       <c r="E98" s="10"/>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="29"/>
+      <c r="A99" s="25"/>
       <c r="B99" s="5" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="C99" s="11">
         <v>0</v>
@@ -2154,9 +2151,9 @@
       <c r="E99" s="10"/>
     </row>
     <row r="100" spans="1:5">
-      <c r="A100" s="29"/>
+      <c r="A100" s="25"/>
       <c r="B100" s="5" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C100" s="11">
         <v>0</v>
@@ -2167,9 +2164,9 @@
       <c r="E100" s="10"/>
     </row>
     <row r="101" spans="1:5">
-      <c r="A101" s="29"/>
+      <c r="A101" s="25"/>
       <c r="B101" s="5" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="C101" s="11">
         <v>0</v>
@@ -2180,9 +2177,9 @@
       <c r="E101" s="10"/>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="29"/>
+      <c r="A102" s="25"/>
       <c r="B102" s="5" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C102" s="11">
         <v>0</v>
@@ -2193,9 +2190,9 @@
       <c r="E102" s="10"/>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="29"/>
+      <c r="A103" s="25"/>
       <c r="B103" s="5" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="C103" s="11">
         <v>0</v>
@@ -2206,9 +2203,9 @@
       <c r="E103" s="10"/>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="29"/>
+      <c r="A104" s="25"/>
       <c r="B104" s="5" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="C104" s="11">
         <v>0</v>
@@ -2219,9 +2216,9 @@
       <c r="E104" s="10"/>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="29"/>
+      <c r="A105" s="25"/>
       <c r="B105" s="5" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="C105" s="11">
         <v>0</v>
@@ -2232,9 +2229,9 @@
       <c r="E105" s="10"/>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="29"/>
+      <c r="A106" s="25"/>
       <c r="B106" s="5" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C106" s="11">
         <v>0</v>
@@ -2245,9 +2242,9 @@
       <c r="E106" s="10"/>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="29"/>
+      <c r="A107" s="25"/>
       <c r="B107" s="5" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C107" s="11">
         <v>0</v>
@@ -2258,9 +2255,9 @@
       <c r="E107" s="10"/>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="29"/>
+      <c r="A108" s="25"/>
       <c r="B108" s="5" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="C108" s="11">
         <v>0</v>
@@ -2271,9 +2268,9 @@
       <c r="E108" s="10"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="29"/>
+      <c r="A109" s="25"/>
       <c r="B109" s="5" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="C109" s="11">
         <v>0</v>
@@ -2284,9 +2281,11 @@
       <c r="E109" s="10"/>
     </row>
     <row r="110" spans="1:5">
-      <c r="A110" s="29"/>
+      <c r="A110" s="26" t="s">
+        <v>100</v>
+      </c>
       <c r="B110" s="5" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="C110" s="11">
         <v>0</v>
@@ -2297,9 +2296,9 @@
       <c r="E110" s="10"/>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="29"/>
+      <c r="A111" s="26"/>
       <c r="B111" s="5" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="C111" s="11">
         <v>0</v>
@@ -2310,9 +2309,9 @@
       <c r="E111" s="10"/>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="29"/>
+      <c r="A112" s="26"/>
       <c r="B112" s="5" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="C112" s="11">
         <v>0</v>
@@ -2323,9 +2322,9 @@
       <c r="E112" s="10"/>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="29"/>
+      <c r="A113" s="26"/>
       <c r="B113" s="5" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="C113" s="11">
         <v>0</v>
@@ -2336,9 +2335,9 @@
       <c r="E113" s="10"/>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="29"/>
+      <c r="A114" s="26"/>
       <c r="B114" s="5" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C114" s="11">
         <v>0</v>
@@ -2349,9 +2348,9 @@
       <c r="E114" s="10"/>
     </row>
     <row r="115" spans="1:5">
-      <c r="A115" s="29"/>
+      <c r="A115" s="26"/>
       <c r="B115" s="5" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C115" s="11">
         <v>0</v>
@@ -2362,9 +2361,9 @@
       <c r="E115" s="10"/>
     </row>
     <row r="116" spans="1:5">
-      <c r="A116" s="29"/>
+      <c r="A116" s="26"/>
       <c r="B116" s="5" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C116" s="11">
         <v>0</v>
@@ -2375,9 +2374,9 @@
       <c r="E116" s="10"/>
     </row>
     <row r="117" spans="1:5">
-      <c r="A117" s="29"/>
+      <c r="A117" s="26"/>
       <c r="B117" s="5" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C117" s="11">
         <v>0</v>
@@ -2388,9 +2387,9 @@
       <c r="E117" s="10"/>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="29"/>
+      <c r="A118" s="26"/>
       <c r="B118" s="5" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="C118" s="11">
         <v>0</v>
@@ -2401,9 +2400,9 @@
       <c r="E118" s="10"/>
     </row>
     <row r="119" spans="1:5">
-      <c r="A119" s="29"/>
+      <c r="A119" s="26"/>
       <c r="B119" s="5" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="C119" s="11">
         <v>0</v>
@@ -2414,9 +2413,9 @@
       <c r="E119" s="10"/>
     </row>
     <row r="120" spans="1:5">
-      <c r="A120" s="29"/>
+      <c r="A120" s="26"/>
       <c r="B120" s="5" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="C120" s="11">
         <v>0</v>
@@ -2427,9 +2426,9 @@
       <c r="E120" s="10"/>
     </row>
     <row r="121" spans="1:5">
-      <c r="A121" s="29"/>
+      <c r="A121" s="26"/>
       <c r="B121" s="5" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="C121" s="11">
         <v>0</v>
@@ -2440,9 +2439,9 @@
       <c r="E121" s="10"/>
     </row>
     <row r="122" spans="1:5">
-      <c r="A122" s="29"/>
+      <c r="A122" s="26"/>
       <c r="B122" s="5" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C122" s="11">
         <v>0</v>
@@ -2453,9 +2452,9 @@
       <c r="E122" s="10"/>
     </row>
     <row r="123" spans="1:5">
-      <c r="A123" s="29"/>
+      <c r="A123" s="26"/>
       <c r="B123" s="5" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="C123" s="11">
         <v>0</v>
@@ -2466,9 +2465,9 @@
       <c r="E123" s="10"/>
     </row>
     <row r="124" spans="1:5">
-      <c r="A124" s="29"/>
+      <c r="A124" s="26"/>
       <c r="B124" s="5" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="C124" s="11">
         <v>0</v>
@@ -2479,9 +2478,9 @@
       <c r="E124" s="10"/>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="29"/>
+      <c r="A125" s="26"/>
       <c r="B125" s="5" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C125" s="11">
         <v>0</v>
@@ -2492,9 +2491,9 @@
       <c r="E125" s="10"/>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" s="29"/>
+      <c r="A126" s="26"/>
       <c r="B126" s="5" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="C126" s="11">
         <v>0</v>
@@ -2505,9 +2504,9 @@
       <c r="E126" s="10"/>
     </row>
     <row r="127" spans="1:5">
-      <c r="A127" s="29"/>
+      <c r="A127" s="26"/>
       <c r="B127" s="5" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="C127" s="11">
         <v>0</v>
@@ -2518,9 +2517,9 @@
       <c r="E127" s="10"/>
     </row>
     <row r="128" spans="1:5">
-      <c r="A128" s="29"/>
+      <c r="A128" s="26"/>
       <c r="B128" s="5" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="C128" s="11">
         <v>0</v>
@@ -2531,9 +2530,9 @@
       <c r="E128" s="10"/>
     </row>
     <row r="129" spans="1:5">
-      <c r="A129" s="29"/>
+      <c r="A129" s="26"/>
       <c r="B129" s="5" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="C129" s="11">
         <v>0</v>
@@ -2544,9 +2543,9 @@
       <c r="E129" s="10"/>
     </row>
     <row r="130" spans="1:5">
-      <c r="A130" s="29"/>
+      <c r="A130" s="26"/>
       <c r="B130" s="5" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="C130" s="11">
         <v>0</v>
@@ -2557,11 +2556,9 @@
       <c r="E130" s="10"/>
     </row>
     <row r="131" spans="1:5">
-      <c r="A131" s="30" t="s">
-        <v>101</v>
-      </c>
+      <c r="A131" s="26"/>
       <c r="B131" s="5" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C131" s="11">
         <v>0</v>
@@ -2572,9 +2569,9 @@
       <c r="E131" s="10"/>
     </row>
     <row r="132" spans="1:5">
-      <c r="A132" s="30"/>
+      <c r="A132" s="26"/>
       <c r="B132" s="5" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C132" s="11">
         <v>0</v>
@@ -2585,9 +2582,9 @@
       <c r="E132" s="10"/>
     </row>
     <row r="133" spans="1:5">
-      <c r="A133" s="30"/>
+      <c r="A133" s="26"/>
       <c r="B133" s="5" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C133" s="11">
         <v>0</v>
@@ -2598,9 +2595,9 @@
       <c r="E133" s="10"/>
     </row>
     <row r="134" spans="1:5">
-      <c r="A134" s="30"/>
+      <c r="A134" s="26"/>
       <c r="B134" s="5" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C134" s="11">
         <v>0</v>
@@ -2611,9 +2608,9 @@
       <c r="E134" s="10"/>
     </row>
     <row r="135" spans="1:5">
-      <c r="A135" s="30"/>
+      <c r="A135" s="26"/>
       <c r="B135" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C135" s="11">
         <v>0</v>
@@ -2624,9 +2621,9 @@
       <c r="E135" s="10"/>
     </row>
     <row r="136" spans="1:5">
-      <c r="A136" s="30"/>
+      <c r="A136" s="26"/>
       <c r="B136" s="5" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="C136" s="11">
         <v>0</v>
@@ -2637,9 +2634,9 @@
       <c r="E136" s="10"/>
     </row>
     <row r="137" spans="1:5">
-      <c r="A137" s="30"/>
+      <c r="A137" s="26"/>
       <c r="B137" s="5" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C137" s="11">
         <v>0</v>
@@ -2650,9 +2647,9 @@
       <c r="E137" s="10"/>
     </row>
     <row r="138" spans="1:5">
-      <c r="A138" s="30"/>
+      <c r="A138" s="26"/>
       <c r="B138" s="5" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C138" s="11">
         <v>0</v>
@@ -2663,9 +2660,9 @@
       <c r="E138" s="10"/>
     </row>
     <row r="139" spans="1:5">
-      <c r="A139" s="30"/>
+      <c r="A139" s="26"/>
       <c r="B139" s="5" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="C139" s="11">
         <v>0</v>
@@ -2676,9 +2673,9 @@
       <c r="E139" s="10"/>
     </row>
     <row r="140" spans="1:5">
-      <c r="A140" s="30"/>
+      <c r="A140" s="26"/>
       <c r="B140" s="5" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C140" s="11">
         <v>0</v>
@@ -2689,9 +2686,9 @@
       <c r="E140" s="10"/>
     </row>
     <row r="141" spans="1:5">
-      <c r="A141" s="30"/>
+      <c r="A141" s="26"/>
       <c r="B141" s="5" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C141" s="11">
         <v>0</v>
@@ -2702,9 +2699,9 @@
       <c r="E141" s="10"/>
     </row>
     <row r="142" spans="1:5">
-      <c r="A142" s="30"/>
+      <c r="A142" s="26"/>
       <c r="B142" s="5" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C142" s="11">
         <v>0</v>
@@ -2715,9 +2712,9 @@
       <c r="E142" s="10"/>
     </row>
     <row r="143" spans="1:5">
-      <c r="A143" s="30"/>
+      <c r="A143" s="26"/>
       <c r="B143" s="5" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C143" s="11">
         <v>0</v>
@@ -2728,9 +2725,9 @@
       <c r="E143" s="10"/>
     </row>
     <row r="144" spans="1:5">
-      <c r="A144" s="30"/>
+      <c r="A144" s="26"/>
       <c r="B144" s="5" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C144" s="11">
         <v>0</v>
@@ -2741,9 +2738,9 @@
       <c r="E144" s="10"/>
     </row>
     <row r="145" spans="1:5">
-      <c r="A145" s="30"/>
+      <c r="A145" s="26"/>
       <c r="B145" s="5" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C145" s="11">
         <v>0</v>
@@ -2754,9 +2751,9 @@
       <c r="E145" s="10"/>
     </row>
     <row r="146" spans="1:5">
-      <c r="A146" s="30"/>
+      <c r="A146" s="26"/>
       <c r="B146" s="5" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C146" s="11">
         <v>0</v>
@@ -2767,9 +2764,9 @@
       <c r="E146" s="10"/>
     </row>
     <row r="147" spans="1:5">
-      <c r="A147" s="30"/>
+      <c r="A147" s="26"/>
       <c r="B147" s="5" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C147" s="11">
         <v>0</v>
@@ -2780,9 +2777,9 @@
       <c r="E147" s="10"/>
     </row>
     <row r="148" spans="1:5">
-      <c r="A148" s="30"/>
+      <c r="A148" s="26"/>
       <c r="B148" s="5" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C148" s="11">
         <v>0</v>
@@ -2793,9 +2790,9 @@
       <c r="E148" s="10"/>
     </row>
     <row r="149" spans="1:5">
-      <c r="A149" s="30"/>
+      <c r="A149" s="26"/>
       <c r="B149" s="5" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C149" s="11">
         <v>0</v>
@@ -2806,9 +2803,9 @@
       <c r="E149" s="10"/>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="30"/>
+      <c r="A150" s="26"/>
       <c r="B150" s="5" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="C150" s="11">
         <v>0</v>
@@ -2819,9 +2816,9 @@
       <c r="E150" s="10"/>
     </row>
     <row r="151" spans="1:5">
-      <c r="A151" s="30"/>
+      <c r="A151" s="26"/>
       <c r="B151" s="5" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="C151" s="11">
         <v>0</v>
@@ -2832,9 +2829,9 @@
       <c r="E151" s="10"/>
     </row>
     <row r="152" spans="1:5">
-      <c r="A152" s="30"/>
+      <c r="A152" s="26"/>
       <c r="B152" s="5" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="C152" s="11">
         <v>0</v>
@@ -2845,9 +2842,9 @@
       <c r="E152" s="10"/>
     </row>
     <row r="153" spans="1:5">
-      <c r="A153" s="30"/>
+      <c r="A153" s="26"/>
       <c r="B153" s="5" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="C153" s="11">
         <v>0</v>
@@ -2858,9 +2855,9 @@
       <c r="E153" s="10"/>
     </row>
     <row r="154" spans="1:5">
-      <c r="A154" s="30"/>
+      <c r="A154" s="26"/>
       <c r="B154" s="5" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C154" s="11">
         <v>0</v>
@@ -2871,9 +2868,9 @@
       <c r="E154" s="10"/>
     </row>
     <row r="155" spans="1:5">
-      <c r="A155" s="30"/>
+      <c r="A155" s="26"/>
       <c r="B155" s="5" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="C155" s="11">
         <v>0</v>
@@ -2884,9 +2881,9 @@
       <c r="E155" s="10"/>
     </row>
     <row r="156" spans="1:5">
-      <c r="A156" s="30"/>
+      <c r="A156" s="26"/>
       <c r="B156" s="5" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C156" s="11">
         <v>0</v>
@@ -2897,9 +2894,9 @@
       <c r="E156" s="10"/>
     </row>
     <row r="157" spans="1:5">
-      <c r="A157" s="30"/>
+      <c r="A157" s="26"/>
       <c r="B157" s="5" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="C157" s="11">
         <v>0</v>
@@ -2910,9 +2907,9 @@
       <c r="E157" s="10"/>
     </row>
     <row r="158" spans="1:5">
-      <c r="A158" s="30"/>
+      <c r="A158" s="26"/>
       <c r="B158" s="5" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="C158" s="11">
         <v>0</v>
@@ -2923,9 +2920,9 @@
       <c r="E158" s="10"/>
     </row>
     <row r="159" spans="1:5">
-      <c r="A159" s="30"/>
+      <c r="A159" s="26"/>
       <c r="B159" s="5" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="C159" s="11">
         <v>0</v>
@@ -2936,378 +2933,168 @@
       <c r="E159" s="10"/>
     </row>
     <row r="160" spans="1:5">
-      <c r="A160" s="30"/>
+      <c r="A160" s="26"/>
       <c r="B160" s="5" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C160" s="11">
         <v>0</v>
       </c>
-      <c r="D160" s="12">
+      <c r="D160" s="13">
         <v>0</v>
       </c>
       <c r="E160" s="10"/>
     </row>
     <row r="161" spans="1:5">
-      <c r="A161" s="30"/>
+      <c r="A161" s="26"/>
       <c r="B161" s="5" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C161" s="11">
         <v>0</v>
       </c>
-      <c r="D161" s="12">
+      <c r="D161" s="7">
         <v>0</v>
       </c>
       <c r="E161" s="10"/>
     </row>
     <row r="162" spans="1:5">
-      <c r="A162" s="30"/>
+      <c r="A162" s="26"/>
       <c r="B162" s="5" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="C162" s="11">
         <v>0</v>
       </c>
-      <c r="D162" s="12">
+      <c r="D162" s="7">
         <v>0</v>
       </c>
       <c r="E162" s="10"/>
     </row>
     <row r="163" spans="1:5">
-      <c r="A163" s="30"/>
+      <c r="A163" s="26"/>
       <c r="B163" s="5" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="C163" s="11">
         <v>0</v>
       </c>
-      <c r="D163" s="12">
+      <c r="D163" s="7">
         <v>0</v>
       </c>
       <c r="E163" s="10"/>
     </row>
     <row r="164" spans="1:5">
-      <c r="A164" s="30"/>
-      <c r="B164" s="5" t="s">
-        <v>80</v>
+      <c r="B164" s="9" t="s">
+        <v>101</v>
       </c>
-      <c r="C164" s="11">
-        <v>0</v>
-      </c>
-      <c r="D164" s="12">
-        <v>0</v>
-      </c>
-      <c r="E164" s="10"/>
+      <c r="C164" s="11"/>
+      <c r="D164" s="7"/>
+      <c r="E164" s="14"/>
     </row>
     <row r="165" spans="1:5">
-      <c r="A165" s="30"/>
-      <c r="B165" s="5" t="s">
-        <v>81</v>
+      <c r="B165" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="C165" s="11">
-        <v>0</v>
+        <f>SUM(C7:C163)</f>
+        <v>20</v>
       </c>
-      <c r="D165" s="12">
-        <v>0</v>
+      <c r="D165" s="11">
+        <f>SUM(D7:D163)</f>
+        <v>46</v>
       </c>
       <c r="E165" s="10"/>
     </row>
     <row r="166" spans="1:5">
-      <c r="A166" s="30"/>
-      <c r="B166" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C166" s="11">
-        <v>0</v>
-      </c>
-      <c r="D166" s="12">
-        <v>0</v>
-      </c>
-      <c r="E166" s="10"/>
+      <c r="B166" s="16"/>
+      <c r="C166" s="17"/>
+      <c r="E166" s="18"/>
     </row>
     <row r="167" spans="1:5">
-      <c r="A167" s="30"/>
-      <c r="B167" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C167" s="11">
-        <v>0</v>
-      </c>
-      <c r="D167" s="12">
-        <v>0</v>
-      </c>
-      <c r="E167" s="10"/>
+      <c r="B167" s="19"/>
+      <c r="C167" s="20"/>
+      <c r="E167" s="21"/>
     </row>
     <row r="168" spans="1:5">
-      <c r="A168" s="30"/>
-      <c r="B168" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C168" s="11">
-        <v>0</v>
-      </c>
-      <c r="D168" s="12">
-        <v>0</v>
-      </c>
-      <c r="E168" s="10"/>
+      <c r="B168" s="19"/>
+      <c r="C168" s="20"/>
+      <c r="E168" s="21"/>
     </row>
     <row r="169" spans="1:5">
-      <c r="A169" s="30"/>
-      <c r="B169" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C169" s="11">
-        <v>0</v>
-      </c>
-      <c r="D169" s="12">
-        <v>0</v>
-      </c>
-      <c r="E169" s="10"/>
+      <c r="B169" s="19"/>
+      <c r="C169" s="20"/>
+      <c r="E169" s="21"/>
     </row>
     <row r="170" spans="1:5">
-      <c r="A170" s="30"/>
-      <c r="B170" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C170" s="11">
-        <v>0</v>
-      </c>
-      <c r="D170" s="12">
-        <v>0</v>
-      </c>
-      <c r="E170" s="10"/>
+      <c r="B170" s="19"/>
+      <c r="C170" s="20"/>
+      <c r="E170" s="21"/>
     </row>
     <row r="171" spans="1:5">
-      <c r="A171" s="30"/>
-      <c r="B171" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C171" s="11">
-        <v>0</v>
-      </c>
-      <c r="D171" s="12">
-        <v>0</v>
-      </c>
-      <c r="E171" s="10"/>
+      <c r="E171" s="22"/>
     </row>
     <row r="172" spans="1:5">
-      <c r="A172" s="30"/>
-      <c r="B172" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C172" s="11">
-        <v>0</v>
-      </c>
-      <c r="D172" s="12">
-        <v>0</v>
-      </c>
-      <c r="E172" s="10"/>
+      <c r="E172" s="22"/>
     </row>
     <row r="173" spans="1:5">
-      <c r="A173" s="30"/>
-      <c r="B173" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C173" s="11">
-        <v>0</v>
-      </c>
-      <c r="D173" s="12">
-        <v>0</v>
-      </c>
-      <c r="E173" s="10"/>
+      <c r="E173" s="22"/>
     </row>
     <row r="174" spans="1:5">
-      <c r="A174" s="30"/>
-      <c r="B174" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C174" s="11">
-        <v>0</v>
-      </c>
-      <c r="D174" s="12">
-        <v>0</v>
-      </c>
-      <c r="E174" s="10"/>
+      <c r="E174" s="22"/>
     </row>
     <row r="175" spans="1:5">
-      <c r="A175" s="30"/>
-      <c r="B175" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C175" s="11">
-        <v>0</v>
-      </c>
-      <c r="D175" s="12">
-        <v>0</v>
-      </c>
-      <c r="E175" s="10"/>
+      <c r="E175" s="22"/>
     </row>
     <row r="176" spans="1:5">
-      <c r="A176" s="30"/>
-      <c r="B176" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C176" s="11">
-        <v>0</v>
-      </c>
-      <c r="D176" s="12">
-        <v>0</v>
-      </c>
-      <c r="E176" s="10"/>
-    </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="30"/>
-      <c r="B177" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C177" s="11">
-        <v>0</v>
-      </c>
-      <c r="D177" s="12">
-        <v>0</v>
-      </c>
-      <c r="E177" s="10"/>
-    </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="30"/>
-      <c r="B178" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C178" s="11">
-        <v>0</v>
-      </c>
-      <c r="D178" s="12">
-        <v>0</v>
-      </c>
-      <c r="E178" s="10"/>
-    </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="30"/>
-      <c r="B179" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C179" s="11">
-        <v>0</v>
-      </c>
-      <c r="D179" s="12">
-        <v>0</v>
-      </c>
-      <c r="E179" s="10"/>
-    </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="30"/>
-      <c r="B180" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C180" s="11">
-        <v>0</v>
-      </c>
-      <c r="D180" s="12">
-        <v>0</v>
-      </c>
-      <c r="E180" s="10"/>
-    </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="30"/>
-      <c r="B181" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C181" s="11">
-        <v>0</v>
-      </c>
-      <c r="D181" s="13">
-        <v>0</v>
-      </c>
-      <c r="E181" s="10"/>
-    </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="30"/>
-      <c r="B182" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C182" s="11">
-        <v>0</v>
-      </c>
-      <c r="D182" s="7">
-        <v>0</v>
-      </c>
-      <c r="E182" s="10"/>
-    </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="30"/>
-      <c r="B183" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C183" s="11">
-        <v>0</v>
-      </c>
-      <c r="D183" s="7">
-        <v>0</v>
-      </c>
-      <c r="E183" s="10"/>
-    </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="30"/>
-      <c r="B184" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C184" s="11">
-        <v>0</v>
-      </c>
-      <c r="D184" s="7">
-        <v>0</v>
-      </c>
-      <c r="E184" s="10"/>
-    </row>
-    <row r="185" spans="1:5">
-      <c r="B185" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C185" s="11"/>
-      <c r="D185" s="7"/>
-      <c r="E185" s="14"/>
-    </row>
-    <row r="186" spans="1:5">
-      <c r="B186" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C186" s="11">
-        <f>SUM(C7:C184)</f>
-        <v>20</v>
-      </c>
-      <c r="D186" s="11">
-        <f>SUM(D7:D184)</f>
-        <v>46</v>
-      </c>
-      <c r="E186" s="10"/>
-    </row>
-    <row r="187" spans="1:5">
-      <c r="B187" s="16"/>
-      <c r="C187" s="17"/>
-      <c r="E187" s="18"/>
-    </row>
-    <row r="188" spans="1:5">
-      <c r="B188" s="19"/>
-      <c r="C188" s="20"/>
-      <c r="E188" s="21"/>
-    </row>
-    <row r="189" spans="1:5">
-      <c r="B189" s="19"/>
-      <c r="C189" s="20"/>
-      <c r="E189" s="21"/>
-    </row>
-    <row r="190" spans="1:5">
-      <c r="B190" s="19"/>
-      <c r="C190" s="20"/>
-      <c r="E190" s="21"/>
-    </row>
-    <row r="191" spans="1:5">
-      <c r="B191" s="19"/>
-      <c r="C191" s="20"/>
-      <c r="E191" s="21"/>
-    </row>
-    <row r="192" spans="1:5">
+      <c r="E176" s="22"/>
+    </row>
+    <row r="177" spans="5:5">
+      <c r="E177" s="22"/>
+    </row>
+    <row r="178" spans="5:5">
+      <c r="E178" s="22"/>
+    </row>
+    <row r="179" spans="5:5">
+      <c r="E179" s="22"/>
+    </row>
+    <row r="180" spans="5:5">
+      <c r="E180" s="22"/>
+    </row>
+    <row r="181" spans="5:5">
+      <c r="E181" s="22"/>
+    </row>
+    <row r="182" spans="5:5">
+      <c r="E182" s="22"/>
+    </row>
+    <row r="183" spans="5:5">
+      <c r="E183" s="22"/>
+    </row>
+    <row r="184" spans="5:5">
+      <c r="E184" s="22"/>
+    </row>
+    <row r="185" spans="5:5">
+      <c r="E185" s="22"/>
+    </row>
+    <row r="186" spans="5:5">
+      <c r="E186" s="22"/>
+    </row>
+    <row r="187" spans="5:5">
+      <c r="E187" s="22"/>
+    </row>
+    <row r="188" spans="5:5">
+      <c r="E188" s="22"/>
+    </row>
+    <row r="189" spans="5:5">
+      <c r="E189" s="22"/>
+    </row>
+    <row r="190" spans="5:5">
+      <c r="E190" s="22"/>
+    </row>
+    <row r="191" spans="5:5">
+      <c r="E191" s="22"/>
+    </row>
+    <row r="192" spans="5:5">
       <c r="E192" s="22"/>
     </row>
     <row r="193" spans="5:5">
@@ -49312,79 +49099,16 @@
     <row r="15526" spans="5:5">
       <c r="E15526" s="22"/>
     </row>
-    <row r="15527" spans="5:5">
-      <c r="E15527" s="22"/>
-    </row>
-    <row r="15528" spans="5:5">
-      <c r="E15528" s="22"/>
-    </row>
-    <row r="15529" spans="5:5">
-      <c r="E15529" s="22"/>
-    </row>
-    <row r="15530" spans="5:5">
-      <c r="E15530" s="22"/>
-    </row>
-    <row r="15531" spans="5:5">
-      <c r="E15531" s="22"/>
-    </row>
-    <row r="15532" spans="5:5">
-      <c r="E15532" s="22"/>
-    </row>
-    <row r="15533" spans="5:5">
-      <c r="E15533" s="22"/>
-    </row>
-    <row r="15534" spans="5:5">
-      <c r="E15534" s="22"/>
-    </row>
-    <row r="15535" spans="5:5">
-      <c r="E15535" s="22"/>
-    </row>
-    <row r="15536" spans="5:5">
-      <c r="E15536" s="22"/>
-    </row>
-    <row r="15537" spans="5:5">
-      <c r="E15537" s="22"/>
-    </row>
-    <row r="15538" spans="5:5">
-      <c r="E15538" s="22"/>
-    </row>
-    <row r="15539" spans="5:5">
-      <c r="E15539" s="22"/>
-    </row>
-    <row r="15540" spans="5:5">
-      <c r="E15540" s="22"/>
-    </row>
-    <row r="15541" spans="5:5">
-      <c r="E15541" s="22"/>
-    </row>
-    <row r="15542" spans="5:5">
-      <c r="E15542" s="22"/>
-    </row>
-    <row r="15543" spans="5:5">
-      <c r="E15543" s="22"/>
-    </row>
-    <row r="15544" spans="5:5">
-      <c r="E15544" s="22"/>
-    </row>
-    <row r="15545" spans="5:5">
-      <c r="E15545" s="22"/>
-    </row>
-    <row r="15546" spans="5:5">
-      <c r="E15546" s="22"/>
-    </row>
-    <row r="15547" spans="5:5">
-      <c r="E15547" s="22"/>
-    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A35:A46"/>
-    <mergeCell ref="A47:A76"/>
-    <mergeCell ref="A77:A130"/>
-    <mergeCell ref="A131:A184"/>
-    <mergeCell ref="A31:A34"/>
     <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A26"/>
-    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A11:A25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A34:A45"/>
+    <mergeCell ref="A46:A55"/>
+    <mergeCell ref="A56:A109"/>
+    <mergeCell ref="A110:A163"/>
+    <mergeCell ref="A30:A33"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
warna blue pink ga ada order jadi hapus semua
</commit_message>
<xml_diff>
--- a/kamila_sarimbit shafeeya.xlsx
+++ b/kamila_sarimbit shafeeya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\sarimbit-shafeeya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74B4A53-A26C-47AF-950D-4EDB57544EE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF842C1-FB6C-43BA-A900-752B3752CDAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="102">
   <si>
     <t>Timestamp</t>
   </si>
@@ -327,9 +327,6 @@
     <t>Koko Ayah Lengan Panjang manset kancing - 3XL</t>
   </si>
   <si>
-    <t>blue - pink</t>
-  </si>
-  <si>
     <t>ruby</t>
   </si>
   <si>
@@ -375,7 +372,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,12 +412,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF6D2C1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF64EAE5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,7 +521,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -597,9 +588,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -889,9 +877,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:E15526"/>
+  <dimension ref="A3:E15472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
       <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
@@ -940,7 +928,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="28"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -953,7 +941,7 @@
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="28"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
@@ -966,7 +954,7 @@
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="28"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
@@ -979,7 +967,7 @@
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="28"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -992,7 +980,7 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="29"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1005,7 +993,7 @@
       <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="29"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1018,7 +1006,7 @@
       <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="29"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1031,7 +1019,7 @@
       <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="29"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1044,7 +1032,7 @@
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="29"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
@@ -1057,7 +1045,7 @@
       <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="29"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -1070,7 +1058,7 @@
       <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="29"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1083,7 +1071,7 @@
       <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="29"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1096,7 +1084,7 @@
       <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="29"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
@@ -1109,7 +1097,7 @@
       <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="29"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1122,7 +1110,7 @@
       <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="29"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
@@ -1135,7 +1123,7 @@
       <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="29"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="5" t="s">
         <v>22</v>
       </c>
@@ -1148,7 +1136,7 @@
       <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="29"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
@@ -1161,7 +1149,7 @@
       <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="29"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
@@ -1174,7 +1162,7 @@
       <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="29"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
@@ -1187,7 +1175,7 @@
       <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="30"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="5" t="s">
         <v>26</v>
       </c>
@@ -1200,7 +1188,7 @@
       <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="30"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="5" t="s">
         <v>27</v>
       </c>
@@ -1213,7 +1201,7 @@
       <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="30"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="5" t="s">
         <v>28</v>
       </c>
@@ -1226,7 +1214,7 @@
       <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="30"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="5" t="s">
         <v>29</v>
       </c>
@@ -1239,7 +1227,7 @@
       <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="27"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="5" t="s">
         <v>30</v>
       </c>
@@ -1252,7 +1240,7 @@
       <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="27"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
@@ -1265,7 +1253,7 @@
       <c r="E31" s="10"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="27"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
@@ -1278,7 +1266,7 @@
       <c r="E32" s="10"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="27"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="5" t="s">
         <v>33</v>
       </c>
@@ -2236,7 +2224,7 @@
       <c r="C106" s="11">
         <v>0</v>
       </c>
-      <c r="D106" s="12">
+      <c r="D106" s="13">
         <v>0</v>
       </c>
       <c r="E106" s="10"/>
@@ -2249,7 +2237,7 @@
       <c r="C107" s="11">
         <v>0</v>
       </c>
-      <c r="D107" s="12">
+      <c r="D107" s="7">
         <v>0</v>
       </c>
       <c r="E107" s="10"/>
@@ -2262,7 +2250,7 @@
       <c r="C108" s="11">
         <v>0</v>
       </c>
-      <c r="D108" s="12">
+      <c r="D108" s="7">
         <v>0</v>
       </c>
       <c r="E108" s="10"/>
@@ -2275,778 +2263,236 @@
       <c r="C109" s="11">
         <v>0</v>
       </c>
-      <c r="D109" s="12">
+      <c r="D109" s="7">
         <v>0</v>
       </c>
       <c r="E109" s="10"/>
     </row>
     <row r="110" spans="1:5">
-      <c r="A110" s="26" t="s">
+      <c r="B110" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="C110" s="11"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="14"/>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="B111" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C111" s="11">
+        <f>SUM(C7:C109)</f>
+        <v>20</v>
+      </c>
+      <c r="D111" s="11">
+        <f>SUM(D7:D109)</f>
         <v>46</v>
       </c>
-      <c r="C110" s="11">
-        <v>0</v>
-      </c>
-      <c r="D110" s="12">
-        <v>0</v>
-      </c>
-      <c r="E110" s="10"/>
-    </row>
-    <row r="111" spans="1:5">
-      <c r="A111" s="26"/>
-      <c r="B111" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C111" s="11">
-        <v>0</v>
-      </c>
-      <c r="D111" s="12">
-        <v>0</v>
-      </c>
       <c r="E111" s="10"/>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="26"/>
-      <c r="B112" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C112" s="11">
-        <v>0</v>
-      </c>
-      <c r="D112" s="12">
-        <v>0</v>
-      </c>
-      <c r="E112" s="10"/>
-    </row>
-    <row r="113" spans="1:5">
-      <c r="A113" s="26"/>
-      <c r="B113" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C113" s="11">
-        <v>0</v>
-      </c>
-      <c r="D113" s="12">
-        <v>0</v>
-      </c>
-      <c r="E113" s="10"/>
-    </row>
-    <row r="114" spans="1:5">
-      <c r="A114" s="26"/>
-      <c r="B114" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C114" s="11">
-        <v>0</v>
-      </c>
-      <c r="D114" s="12">
-        <v>0</v>
-      </c>
-      <c r="E114" s="10"/>
-    </row>
-    <row r="115" spans="1:5">
-      <c r="A115" s="26"/>
-      <c r="B115" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C115" s="11">
-        <v>0</v>
-      </c>
-      <c r="D115" s="12">
-        <v>0</v>
-      </c>
-      <c r="E115" s="10"/>
-    </row>
-    <row r="116" spans="1:5">
-      <c r="A116" s="26"/>
-      <c r="B116" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C116" s="11">
-        <v>0</v>
-      </c>
-      <c r="D116" s="12">
-        <v>0</v>
-      </c>
-      <c r="E116" s="10"/>
-    </row>
-    <row r="117" spans="1:5">
-      <c r="A117" s="26"/>
-      <c r="B117" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C117" s="11">
-        <v>0</v>
-      </c>
-      <c r="D117" s="12">
-        <v>0</v>
-      </c>
-      <c r="E117" s="10"/>
-    </row>
-    <row r="118" spans="1:5">
-      <c r="A118" s="26"/>
-      <c r="B118" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C118" s="11">
-        <v>0</v>
-      </c>
-      <c r="D118" s="12">
-        <v>0</v>
-      </c>
-      <c r="E118" s="10"/>
-    </row>
-    <row r="119" spans="1:5">
-      <c r="A119" s="26"/>
-      <c r="B119" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C119" s="11">
-        <v>0</v>
-      </c>
-      <c r="D119" s="12">
-        <v>0</v>
-      </c>
-      <c r="E119" s="10"/>
-    </row>
-    <row r="120" spans="1:5">
-      <c r="A120" s="26"/>
-      <c r="B120" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C120" s="11">
-        <v>0</v>
-      </c>
-      <c r="D120" s="12">
-        <v>0</v>
-      </c>
-      <c r="E120" s="10"/>
-    </row>
-    <row r="121" spans="1:5">
-      <c r="A121" s="26"/>
-      <c r="B121" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C121" s="11">
-        <v>0</v>
-      </c>
-      <c r="D121" s="12">
-        <v>0</v>
-      </c>
-      <c r="E121" s="10"/>
-    </row>
-    <row r="122" spans="1:5">
-      <c r="A122" s="26"/>
-      <c r="B122" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C122" s="11">
-        <v>0</v>
-      </c>
-      <c r="D122" s="12">
-        <v>0</v>
-      </c>
-      <c r="E122" s="10"/>
-    </row>
-    <row r="123" spans="1:5">
-      <c r="A123" s="26"/>
-      <c r="B123" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C123" s="11">
-        <v>0</v>
-      </c>
-      <c r="D123" s="12">
-        <v>0</v>
-      </c>
-      <c r="E123" s="10"/>
-    </row>
-    <row r="124" spans="1:5">
-      <c r="A124" s="26"/>
-      <c r="B124" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C124" s="11">
-        <v>0</v>
-      </c>
-      <c r="D124" s="12">
-        <v>0</v>
-      </c>
-      <c r="E124" s="10"/>
-    </row>
-    <row r="125" spans="1:5">
-      <c r="A125" s="26"/>
-      <c r="B125" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C125" s="11">
-        <v>0</v>
-      </c>
-      <c r="D125" s="12">
-        <v>0</v>
-      </c>
-      <c r="E125" s="10"/>
-    </row>
-    <row r="126" spans="1:5">
-      <c r="A126" s="26"/>
-      <c r="B126" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C126" s="11">
-        <v>0</v>
-      </c>
-      <c r="D126" s="12">
-        <v>0</v>
-      </c>
-      <c r="E126" s="10"/>
-    </row>
-    <row r="127" spans="1:5">
-      <c r="A127" s="26"/>
-      <c r="B127" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C127" s="11">
-        <v>0</v>
-      </c>
-      <c r="D127" s="12">
-        <v>0</v>
-      </c>
-      <c r="E127" s="10"/>
-    </row>
-    <row r="128" spans="1:5">
-      <c r="A128" s="26"/>
-      <c r="B128" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C128" s="11">
-        <v>0</v>
-      </c>
-      <c r="D128" s="12">
-        <v>0</v>
-      </c>
-      <c r="E128" s="10"/>
-    </row>
-    <row r="129" spans="1:5">
-      <c r="A129" s="26"/>
-      <c r="B129" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C129" s="11">
-        <v>0</v>
-      </c>
-      <c r="D129" s="12">
-        <v>0</v>
-      </c>
-      <c r="E129" s="10"/>
-    </row>
-    <row r="130" spans="1:5">
-      <c r="A130" s="26"/>
-      <c r="B130" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C130" s="11">
-        <v>0</v>
-      </c>
-      <c r="D130" s="12">
-        <v>0</v>
-      </c>
-      <c r="E130" s="10"/>
-    </row>
-    <row r="131" spans="1:5">
-      <c r="A131" s="26"/>
-      <c r="B131" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C131" s="11">
-        <v>0</v>
-      </c>
-      <c r="D131" s="12">
-        <v>0</v>
-      </c>
-      <c r="E131" s="10"/>
-    </row>
-    <row r="132" spans="1:5">
-      <c r="A132" s="26"/>
-      <c r="B132" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C132" s="11">
-        <v>0</v>
-      </c>
-      <c r="D132" s="12">
-        <v>0</v>
-      </c>
-      <c r="E132" s="10"/>
-    </row>
-    <row r="133" spans="1:5">
-      <c r="A133" s="26"/>
-      <c r="B133" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C133" s="11">
-        <v>0</v>
-      </c>
-      <c r="D133" s="12">
-        <v>0</v>
-      </c>
-      <c r="E133" s="10"/>
-    </row>
-    <row r="134" spans="1:5">
-      <c r="A134" s="26"/>
-      <c r="B134" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C134" s="11">
-        <v>0</v>
-      </c>
-      <c r="D134" s="12">
-        <v>0</v>
-      </c>
-      <c r="E134" s="10"/>
-    </row>
-    <row r="135" spans="1:5">
-      <c r="A135" s="26"/>
-      <c r="B135" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C135" s="11">
-        <v>0</v>
-      </c>
-      <c r="D135" s="12">
-        <v>0</v>
-      </c>
-      <c r="E135" s="10"/>
-    </row>
-    <row r="136" spans="1:5">
-      <c r="A136" s="26"/>
-      <c r="B136" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C136" s="11">
-        <v>0</v>
-      </c>
-      <c r="D136" s="12">
-        <v>0</v>
-      </c>
-      <c r="E136" s="10"/>
-    </row>
-    <row r="137" spans="1:5">
-      <c r="A137" s="26"/>
-      <c r="B137" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C137" s="11">
-        <v>0</v>
-      </c>
-      <c r="D137" s="12">
-        <v>0</v>
-      </c>
-      <c r="E137" s="10"/>
-    </row>
-    <row r="138" spans="1:5">
-      <c r="A138" s="26"/>
-      <c r="B138" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C138" s="11">
-        <v>0</v>
-      </c>
-      <c r="D138" s="12">
-        <v>0</v>
-      </c>
-      <c r="E138" s="10"/>
-    </row>
-    <row r="139" spans="1:5">
-      <c r="A139" s="26"/>
-      <c r="B139" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C139" s="11">
-        <v>0</v>
-      </c>
-      <c r="D139" s="12">
-        <v>0</v>
-      </c>
-      <c r="E139" s="10"/>
-    </row>
-    <row r="140" spans="1:5">
-      <c r="A140" s="26"/>
-      <c r="B140" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C140" s="11">
-        <v>0</v>
-      </c>
-      <c r="D140" s="12">
-        <v>0</v>
-      </c>
-      <c r="E140" s="10"/>
-    </row>
-    <row r="141" spans="1:5">
-      <c r="A141" s="26"/>
-      <c r="B141" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C141" s="11">
-        <v>0</v>
-      </c>
-      <c r="D141" s="12">
-        <v>0</v>
-      </c>
-      <c r="E141" s="10"/>
-    </row>
-    <row r="142" spans="1:5">
-      <c r="A142" s="26"/>
-      <c r="B142" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C142" s="11">
-        <v>0</v>
-      </c>
-      <c r="D142" s="12">
-        <v>0</v>
-      </c>
-      <c r="E142" s="10"/>
-    </row>
-    <row r="143" spans="1:5">
-      <c r="A143" s="26"/>
-      <c r="B143" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C143" s="11">
-        <v>0</v>
-      </c>
-      <c r="D143" s="12">
-        <v>0</v>
-      </c>
-      <c r="E143" s="10"/>
-    </row>
-    <row r="144" spans="1:5">
-      <c r="A144" s="26"/>
-      <c r="B144" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C144" s="11">
-        <v>0</v>
-      </c>
-      <c r="D144" s="12">
-        <v>0</v>
-      </c>
-      <c r="E144" s="10"/>
-    </row>
-    <row r="145" spans="1:5">
-      <c r="A145" s="26"/>
-      <c r="B145" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C145" s="11">
-        <v>0</v>
-      </c>
-      <c r="D145" s="12">
-        <v>0</v>
-      </c>
-      <c r="E145" s="10"/>
-    </row>
-    <row r="146" spans="1:5">
-      <c r="A146" s="26"/>
-      <c r="B146" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C146" s="11">
-        <v>0</v>
-      </c>
-      <c r="D146" s="12">
-        <v>0</v>
-      </c>
-      <c r="E146" s="10"/>
-    </row>
-    <row r="147" spans="1:5">
-      <c r="A147" s="26"/>
-      <c r="B147" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C147" s="11">
-        <v>0</v>
-      </c>
-      <c r="D147" s="12">
-        <v>0</v>
-      </c>
-      <c r="E147" s="10"/>
-    </row>
-    <row r="148" spans="1:5">
-      <c r="A148" s="26"/>
-      <c r="B148" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C148" s="11">
-        <v>0</v>
-      </c>
-      <c r="D148" s="12">
-        <v>0</v>
-      </c>
-      <c r="E148" s="10"/>
-    </row>
-    <row r="149" spans="1:5">
-      <c r="A149" s="26"/>
-      <c r="B149" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C149" s="11">
-        <v>0</v>
-      </c>
-      <c r="D149" s="12">
-        <v>0</v>
-      </c>
-      <c r="E149" s="10"/>
-    </row>
-    <row r="150" spans="1:5">
-      <c r="A150" s="26"/>
-      <c r="B150" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C150" s="11">
-        <v>0</v>
-      </c>
-      <c r="D150" s="12">
-        <v>0</v>
-      </c>
-      <c r="E150" s="10"/>
-    </row>
-    <row r="151" spans="1:5">
-      <c r="A151" s="26"/>
-      <c r="B151" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C151" s="11">
-        <v>0</v>
-      </c>
-      <c r="D151" s="12">
-        <v>0</v>
-      </c>
-      <c r="E151" s="10"/>
-    </row>
-    <row r="152" spans="1:5">
-      <c r="A152" s="26"/>
-      <c r="B152" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C152" s="11">
-        <v>0</v>
-      </c>
-      <c r="D152" s="12">
-        <v>0</v>
-      </c>
-      <c r="E152" s="10"/>
-    </row>
-    <row r="153" spans="1:5">
-      <c r="A153" s="26"/>
-      <c r="B153" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C153" s="11">
-        <v>0</v>
-      </c>
-      <c r="D153" s="12">
-        <v>0</v>
-      </c>
-      <c r="E153" s="10"/>
-    </row>
-    <row r="154" spans="1:5">
-      <c r="A154" s="26"/>
-      <c r="B154" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C154" s="11">
-        <v>0</v>
-      </c>
-      <c r="D154" s="12">
-        <v>0</v>
-      </c>
-      <c r="E154" s="10"/>
-    </row>
-    <row r="155" spans="1:5">
-      <c r="A155" s="26"/>
-      <c r="B155" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C155" s="11">
-        <v>0</v>
-      </c>
-      <c r="D155" s="12">
-        <v>0</v>
-      </c>
-      <c r="E155" s="10"/>
-    </row>
-    <row r="156" spans="1:5">
-      <c r="A156" s="26"/>
-      <c r="B156" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C156" s="11">
-        <v>0</v>
-      </c>
-      <c r="D156" s="12">
-        <v>0</v>
-      </c>
-      <c r="E156" s="10"/>
-    </row>
-    <row r="157" spans="1:5">
-      <c r="A157" s="26"/>
-      <c r="B157" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C157" s="11">
-        <v>0</v>
-      </c>
-      <c r="D157" s="12">
-        <v>0</v>
-      </c>
-      <c r="E157" s="10"/>
-    </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="26"/>
-      <c r="B158" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C158" s="11">
-        <v>0</v>
-      </c>
-      <c r="D158" s="12">
-        <v>0</v>
-      </c>
-      <c r="E158" s="10"/>
-    </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="26"/>
-      <c r="B159" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C159" s="11">
-        <v>0</v>
-      </c>
-      <c r="D159" s="12">
-        <v>0</v>
-      </c>
-      <c r="E159" s="10"/>
-    </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="26"/>
-      <c r="B160" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C160" s="11">
-        <v>0</v>
-      </c>
-      <c r="D160" s="13">
-        <v>0</v>
-      </c>
-      <c r="E160" s="10"/>
-    </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="26"/>
-      <c r="B161" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C161" s="11">
-        <v>0</v>
-      </c>
-      <c r="D161" s="7">
-        <v>0</v>
-      </c>
-      <c r="E161" s="10"/>
-    </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="26"/>
-      <c r="B162" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C162" s="11">
-        <v>0</v>
-      </c>
-      <c r="D162" s="7">
-        <v>0</v>
-      </c>
-      <c r="E162" s="10"/>
-    </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="26"/>
-      <c r="B163" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C163" s="11">
-        <v>0</v>
-      </c>
-      <c r="D163" s="7">
-        <v>0</v>
-      </c>
-      <c r="E163" s="10"/>
-    </row>
-    <row r="164" spans="1:5">
-      <c r="B164" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C164" s="11"/>
-      <c r="D164" s="7"/>
-      <c r="E164" s="14"/>
-    </row>
-    <row r="165" spans="1:5">
-      <c r="B165" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C165" s="11">
-        <f>SUM(C7:C163)</f>
-        <v>20</v>
-      </c>
-      <c r="D165" s="11">
-        <f>SUM(D7:D163)</f>
-        <v>46</v>
-      </c>
-      <c r="E165" s="10"/>
-    </row>
-    <row r="166" spans="1:5">
-      <c r="B166" s="16"/>
-      <c r="C166" s="17"/>
-      <c r="E166" s="18"/>
-    </row>
-    <row r="167" spans="1:5">
-      <c r="B167" s="19"/>
-      <c r="C167" s="20"/>
-      <c r="E167" s="21"/>
-    </row>
-    <row r="168" spans="1:5">
-      <c r="B168" s="19"/>
-      <c r="C168" s="20"/>
-      <c r="E168" s="21"/>
-    </row>
-    <row r="169" spans="1:5">
-      <c r="B169" s="19"/>
-      <c r="C169" s="20"/>
-      <c r="E169" s="21"/>
-    </row>
-    <row r="170" spans="1:5">
-      <c r="B170" s="19"/>
-      <c r="C170" s="20"/>
-      <c r="E170" s="21"/>
-    </row>
-    <row r="171" spans="1:5">
+      <c r="B112" s="16"/>
+      <c r="C112" s="17"/>
+      <c r="E112" s="18"/>
+    </row>
+    <row r="113" spans="2:5">
+      <c r="B113" s="19"/>
+      <c r="C113" s="20"/>
+      <c r="E113" s="21"/>
+    </row>
+    <row r="114" spans="2:5">
+      <c r="B114" s="19"/>
+      <c r="C114" s="20"/>
+      <c r="E114" s="21"/>
+    </row>
+    <row r="115" spans="2:5">
+      <c r="B115" s="19"/>
+      <c r="C115" s="20"/>
+      <c r="E115" s="21"/>
+    </row>
+    <row r="116" spans="2:5">
+      <c r="B116" s="19"/>
+      <c r="C116" s="20"/>
+      <c r="E116" s="21"/>
+    </row>
+    <row r="117" spans="2:5">
+      <c r="E117" s="22"/>
+    </row>
+    <row r="118" spans="2:5">
+      <c r="E118" s="22"/>
+    </row>
+    <row r="119" spans="2:5">
+      <c r="E119" s="22"/>
+    </row>
+    <row r="120" spans="2:5">
+      <c r="E120" s="22"/>
+    </row>
+    <row r="121" spans="2:5">
+      <c r="E121" s="22"/>
+    </row>
+    <row r="122" spans="2:5">
+      <c r="E122" s="22"/>
+    </row>
+    <row r="123" spans="2:5">
+      <c r="E123" s="22"/>
+    </row>
+    <row r="124" spans="2:5">
+      <c r="E124" s="22"/>
+    </row>
+    <row r="125" spans="2:5">
+      <c r="E125" s="22"/>
+    </row>
+    <row r="126" spans="2:5">
+      <c r="E126" s="22"/>
+    </row>
+    <row r="127" spans="2:5">
+      <c r="E127" s="22"/>
+    </row>
+    <row r="128" spans="2:5">
+      <c r="E128" s="22"/>
+    </row>
+    <row r="129" spans="5:5">
+      <c r="E129" s="22"/>
+    </row>
+    <row r="130" spans="5:5">
+      <c r="E130" s="22"/>
+    </row>
+    <row r="131" spans="5:5">
+      <c r="E131" s="22"/>
+    </row>
+    <row r="132" spans="5:5">
+      <c r="E132" s="22"/>
+    </row>
+    <row r="133" spans="5:5">
+      <c r="E133" s="22"/>
+    </row>
+    <row r="134" spans="5:5">
+      <c r="E134" s="22"/>
+    </row>
+    <row r="135" spans="5:5">
+      <c r="E135" s="22"/>
+    </row>
+    <row r="136" spans="5:5">
+      <c r="E136" s="22"/>
+    </row>
+    <row r="137" spans="5:5">
+      <c r="E137" s="22"/>
+    </row>
+    <row r="138" spans="5:5">
+      <c r="E138" s="22"/>
+    </row>
+    <row r="139" spans="5:5">
+      <c r="E139" s="22"/>
+    </row>
+    <row r="140" spans="5:5">
+      <c r="E140" s="22"/>
+    </row>
+    <row r="141" spans="5:5">
+      <c r="E141" s="22"/>
+    </row>
+    <row r="142" spans="5:5">
+      <c r="E142" s="22"/>
+    </row>
+    <row r="143" spans="5:5">
+      <c r="E143" s="22"/>
+    </row>
+    <row r="144" spans="5:5">
+      <c r="E144" s="22"/>
+    </row>
+    <row r="145" spans="5:5">
+      <c r="E145" s="22"/>
+    </row>
+    <row r="146" spans="5:5">
+      <c r="E146" s="22"/>
+    </row>
+    <row r="147" spans="5:5">
+      <c r="E147" s="22"/>
+    </row>
+    <row r="148" spans="5:5">
+      <c r="E148" s="22"/>
+    </row>
+    <row r="149" spans="5:5">
+      <c r="E149" s="22"/>
+    </row>
+    <row r="150" spans="5:5">
+      <c r="E150" s="22"/>
+    </row>
+    <row r="151" spans="5:5">
+      <c r="E151" s="22"/>
+    </row>
+    <row r="152" spans="5:5">
+      <c r="E152" s="22"/>
+    </row>
+    <row r="153" spans="5:5">
+      <c r="E153" s="22"/>
+    </row>
+    <row r="154" spans="5:5">
+      <c r="E154" s="22"/>
+    </row>
+    <row r="155" spans="5:5">
+      <c r="E155" s="22"/>
+    </row>
+    <row r="156" spans="5:5">
+      <c r="E156" s="22"/>
+    </row>
+    <row r="157" spans="5:5">
+      <c r="E157" s="22"/>
+    </row>
+    <row r="158" spans="5:5">
+      <c r="E158" s="22"/>
+    </row>
+    <row r="159" spans="5:5">
+      <c r="E159" s="22"/>
+    </row>
+    <row r="160" spans="5:5">
+      <c r="E160" s="22"/>
+    </row>
+    <row r="161" spans="5:5">
+      <c r="E161" s="22"/>
+    </row>
+    <row r="162" spans="5:5">
+      <c r="E162" s="22"/>
+    </row>
+    <row r="163" spans="5:5">
+      <c r="E163" s="22"/>
+    </row>
+    <row r="164" spans="5:5">
+      <c r="E164" s="22"/>
+    </row>
+    <row r="165" spans="5:5">
+      <c r="E165" s="22"/>
+    </row>
+    <row r="166" spans="5:5">
+      <c r="E166" s="22"/>
+    </row>
+    <row r="167" spans="5:5">
+      <c r="E167" s="22"/>
+    </row>
+    <row r="168" spans="5:5">
+      <c r="E168" s="22"/>
+    </row>
+    <row r="169" spans="5:5">
+      <c r="E169" s="22"/>
+    </row>
+    <row r="170" spans="5:5">
+      <c r="E170" s="22"/>
+    </row>
+    <row r="171" spans="5:5">
       <c r="E171" s="22"/>
     </row>
-    <row r="172" spans="1:5">
+    <row r="172" spans="5:5">
       <c r="E172" s="22"/>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="5:5">
       <c r="E173" s="22"/>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="5:5">
       <c r="E174" s="22"/>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="5:5">
       <c r="E175" s="22"/>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="5:5">
       <c r="E176" s="22"/>
     </row>
     <row r="177" spans="5:5">
@@ -48937,177 +48383,14 @@
     <row r="15472" spans="5:5">
       <c r="E15472" s="22"/>
     </row>
-    <row r="15473" spans="5:5">
-      <c r="E15473" s="22"/>
-    </row>
-    <row r="15474" spans="5:5">
-      <c r="E15474" s="22"/>
-    </row>
-    <row r="15475" spans="5:5">
-      <c r="E15475" s="22"/>
-    </row>
-    <row r="15476" spans="5:5">
-      <c r="E15476" s="22"/>
-    </row>
-    <row r="15477" spans="5:5">
-      <c r="E15477" s="22"/>
-    </row>
-    <row r="15478" spans="5:5">
-      <c r="E15478" s="22"/>
-    </row>
-    <row r="15479" spans="5:5">
-      <c r="E15479" s="22"/>
-    </row>
-    <row r="15480" spans="5:5">
-      <c r="E15480" s="22"/>
-    </row>
-    <row r="15481" spans="5:5">
-      <c r="E15481" s="22"/>
-    </row>
-    <row r="15482" spans="5:5">
-      <c r="E15482" s="22"/>
-    </row>
-    <row r="15483" spans="5:5">
-      <c r="E15483" s="22"/>
-    </row>
-    <row r="15484" spans="5:5">
-      <c r="E15484" s="22"/>
-    </row>
-    <row r="15485" spans="5:5">
-      <c r="E15485" s="22"/>
-    </row>
-    <row r="15486" spans="5:5">
-      <c r="E15486" s="22"/>
-    </row>
-    <row r="15487" spans="5:5">
-      <c r="E15487" s="22"/>
-    </row>
-    <row r="15488" spans="5:5">
-      <c r="E15488" s="22"/>
-    </row>
-    <row r="15489" spans="5:5">
-      <c r="E15489" s="22"/>
-    </row>
-    <row r="15490" spans="5:5">
-      <c r="E15490" s="22"/>
-    </row>
-    <row r="15491" spans="5:5">
-      <c r="E15491" s="22"/>
-    </row>
-    <row r="15492" spans="5:5">
-      <c r="E15492" s="22"/>
-    </row>
-    <row r="15493" spans="5:5">
-      <c r="E15493" s="22"/>
-    </row>
-    <row r="15494" spans="5:5">
-      <c r="E15494" s="22"/>
-    </row>
-    <row r="15495" spans="5:5">
-      <c r="E15495" s="22"/>
-    </row>
-    <row r="15496" spans="5:5">
-      <c r="E15496" s="22"/>
-    </row>
-    <row r="15497" spans="5:5">
-      <c r="E15497" s="22"/>
-    </row>
-    <row r="15498" spans="5:5">
-      <c r="E15498" s="22"/>
-    </row>
-    <row r="15499" spans="5:5">
-      <c r="E15499" s="22"/>
-    </row>
-    <row r="15500" spans="5:5">
-      <c r="E15500" s="22"/>
-    </row>
-    <row r="15501" spans="5:5">
-      <c r="E15501" s="22"/>
-    </row>
-    <row r="15502" spans="5:5">
-      <c r="E15502" s="22"/>
-    </row>
-    <row r="15503" spans="5:5">
-      <c r="E15503" s="22"/>
-    </row>
-    <row r="15504" spans="5:5">
-      <c r="E15504" s="22"/>
-    </row>
-    <row r="15505" spans="5:5">
-      <c r="E15505" s="22"/>
-    </row>
-    <row r="15506" spans="5:5">
-      <c r="E15506" s="22"/>
-    </row>
-    <row r="15507" spans="5:5">
-      <c r="E15507" s="22"/>
-    </row>
-    <row r="15508" spans="5:5">
-      <c r="E15508" s="22"/>
-    </row>
-    <row r="15509" spans="5:5">
-      <c r="E15509" s="22"/>
-    </row>
-    <row r="15510" spans="5:5">
-      <c r="E15510" s="22"/>
-    </row>
-    <row r="15511" spans="5:5">
-      <c r="E15511" s="22"/>
-    </row>
-    <row r="15512" spans="5:5">
-      <c r="E15512" s="22"/>
-    </row>
-    <row r="15513" spans="5:5">
-      <c r="E15513" s="22"/>
-    </row>
-    <row r="15514" spans="5:5">
-      <c r="E15514" s="22"/>
-    </row>
-    <row r="15515" spans="5:5">
-      <c r="E15515" s="22"/>
-    </row>
-    <row r="15516" spans="5:5">
-      <c r="E15516" s="22"/>
-    </row>
-    <row r="15517" spans="5:5">
-      <c r="E15517" s="22"/>
-    </row>
-    <row r="15518" spans="5:5">
-      <c r="E15518" s="22"/>
-    </row>
-    <row r="15519" spans="5:5">
-      <c r="E15519" s="22"/>
-    </row>
-    <row r="15520" spans="5:5">
-      <c r="E15520" s="22"/>
-    </row>
-    <row r="15521" spans="5:5">
-      <c r="E15521" s="22"/>
-    </row>
-    <row r="15522" spans="5:5">
-      <c r="E15522" s="22"/>
-    </row>
-    <row r="15523" spans="5:5">
-      <c r="E15523" s="22"/>
-    </row>
-    <row r="15524" spans="5:5">
-      <c r="E15524" s="22"/>
-    </row>
-    <row r="15525" spans="5:5">
-      <c r="E15525" s="22"/>
-    </row>
-    <row r="15526" spans="5:5">
-      <c r="E15526" s="22"/>
-    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A25"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A34:A45"/>
     <mergeCell ref="A46:A55"/>
     <mergeCell ref="A56:A109"/>
-    <mergeCell ref="A110:A163"/>
     <mergeCell ref="A30:A33"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>